<commit_message>
all logos updated on excil file
</commit_message>
<xml_diff>
--- a/My_application/third_party/PHPExcel/finance/test3.xlsx
+++ b/My_application/third_party/PHPExcel/finance/test3.xlsx
@@ -557,6 +557,49 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>112835</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>2601</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13335000" y="0"/>
+          <a:ext cx="1504950" cy="588755"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -829,7 +872,7 @@
   <dimension ref="A1:K74"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1962,5 +2005,6 @@
   <phoneticPr fontId="22" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0" footer="0"/>
   <pageSetup scale="58" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated excel sheets 7.0
</commit_message>
<xml_diff>
--- a/My_application/third_party/PHPExcel/finance/test3.xlsx
+++ b/My_application/third_party/PHPExcel/finance/test3.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="42">
   <si>
     <t>Cash</t>
   </si>
@@ -152,13 +152,16 @@
     <t>BALANCE SHEET EXCEL</t>
   </si>
   <si>
-    <t>Year 1</t>
-  </si>
-  <si>
     <t>Year 2</t>
   </si>
   <si>
     <t>Currency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Year </t>
+  </si>
+  <si>
+    <t>Others</t>
   </si>
 </sst>
 </file>
@@ -543,14 +546,14 @@
     <xf numFmtId="43" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="43" fontId="13" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="43" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="43" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="13" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="13" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -596,8 +599,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>112835</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>230066</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>2601</xdr:rowOff>
     </xdr:to>
@@ -896,34 +899,36 @@
     <tabColor theme="9" tint="-0.249977111117893"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K74"/>
+  <dimension ref="A1:K75"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.85546875" style="25" customWidth="1"/>
     <col min="2" max="2" width="62.42578125" style="25" customWidth="1"/>
-    <col min="3" max="4" width="20.85546875" style="25" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" style="25" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" style="25" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="6.5703125" style="25" customWidth="1"/>
     <col min="6" max="6" width="62.42578125" style="25" customWidth="1"/>
-    <col min="7" max="8" width="20.85546875" style="25" customWidth="1"/>
+    <col min="7" max="7" width="20.85546875" style="25" customWidth="1"/>
+    <col min="8" max="8" width="20.85546875" style="25" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="5.85546875" style="25" customWidth="1"/>
     <col min="10" max="10" width="4.42578125" style="25" customWidth="1"/>
     <col min="11" max="16384" width="8.85546875" style="25"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:9" s="2" customFormat="1" ht="45.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
       <c r="E1" s="1"/>
       <c r="F1" s="40" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G1" s="41"/>
     </row>
@@ -932,20 +937,20 @@
         <v>4</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>39</v>
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="5" t="s">
         <v>5</v>
       </c>
       <c r="G2" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H2" s="6" t="s">
         <v>38</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="3" spans="2:9" s="14" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -1096,17 +1101,16 @@
       </c>
       <c r="I9" s="13"/>
     </row>
-    <row r="10" spans="2:9" s="14" customFormat="1" ht="24.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:9" s="14" customFormat="1" ht="24.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="45"/>
       <c r="C10" s="45"/>
       <c r="D10" s="45"/>
       <c r="E10" s="10"/>
-      <c r="F10" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="G10" s="21">
-        <f>SUM(G4:G9)</f>
-        <v>10000</v>
+      <c r="F10" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="G10" s="16">
+        <v>0</v>
       </c>
       <c r="H10" s="21">
         <f>SUM(H4:H9)</f>
@@ -1114,16 +1118,21 @@
       </c>
       <c r="I10" s="13"/>
     </row>
-    <row r="11" spans="2:9" s="14" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:9" s="14" customFormat="1" ht="24.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B11" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
       <c r="E11" s="10"/>
-      <c r="F11" s="44"/>
-      <c r="G11" s="44"/>
-      <c r="H11" s="44"/>
+      <c r="F11" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" s="21">
+        <f>SUM(G4:G10)</f>
+        <v>10000</v>
+      </c>
+      <c r="H11" s="42"/>
       <c r="I11" s="13"/>
     </row>
     <row r="12" spans="2:9" s="14" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -1137,10 +1146,8 @@
         <v>0</v>
       </c>
       <c r="E12" s="10"/>
-      <c r="F12" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="G12" s="23"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="42"/>
       <c r="H12" s="23"/>
       <c r="I12" s="13"/>
     </row>
@@ -1155,12 +1162,10 @@
         <v>0</v>
       </c>
       <c r="E13" s="10"/>
-      <c r="F13" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="G13" s="16">
-        <v>3000</v>
-      </c>
+      <c r="F13" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="G13" s="23"/>
       <c r="H13" s="16">
         <v>0</v>
       </c>
@@ -1178,10 +1183,10 @@
       </c>
       <c r="E14" s="10"/>
       <c r="F14" s="17" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="G14" s="16">
-        <v>0</v>
+        <v>3000</v>
       </c>
       <c r="H14" s="16">
         <v>0</v>
@@ -1200,7 +1205,7 @@
       </c>
       <c r="E15" s="10"/>
       <c r="F15" s="17" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="G15" s="16">
         <v>0</v>
@@ -1210,7 +1215,7 @@
       </c>
       <c r="I15" s="13"/>
     </row>
-    <row r="16" spans="2:9" s="14" customFormat="1" ht="24.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:9" s="14" customFormat="1" ht="24.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="18" t="s">
         <v>13</v>
       </c>
@@ -1223,12 +1228,11 @@
         <v>0</v>
       </c>
       <c r="E16" s="10"/>
-      <c r="F16" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="G16" s="21">
-        <f>SUM(G13:G15)</f>
-        <v>3000</v>
+      <c r="F16" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="G16" s="16">
+        <v>0</v>
       </c>
       <c r="H16" s="21">
         <f>SUM(H13:H15)</f>
@@ -1236,14 +1240,19 @@
       </c>
       <c r="I16" s="13"/>
     </row>
-    <row r="17" spans="1:11" s="14" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" s="14" customFormat="1" ht="24.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B17" s="45"/>
       <c r="C17" s="45"/>
       <c r="D17" s="45"/>
       <c r="E17" s="10"/>
-      <c r="F17" s="44"/>
-      <c r="G17" s="44"/>
-      <c r="H17" s="44"/>
+      <c r="F17" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="G17" s="21">
+        <f>SUM(G14:G16)</f>
+        <v>3000</v>
+      </c>
+      <c r="H17" s="42"/>
       <c r="I17" s="13"/>
     </row>
     <row r="18" spans="1:11" s="14" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -1253,10 +1262,8 @@
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
       <c r="E18" s="10"/>
-      <c r="F18" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="G18" s="23"/>
+      <c r="F18" s="42"/>
+      <c r="G18" s="42"/>
       <c r="H18" s="23"/>
       <c r="I18" s="13"/>
     </row>
@@ -1271,12 +1278,10 @@
         <v>0</v>
       </c>
       <c r="E19" s="10"/>
-      <c r="F19" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="G19" s="16">
-        <v>8000</v>
-      </c>
+      <c r="F19" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="G19" s="23"/>
       <c r="H19" s="16">
         <v>0</v>
       </c>
@@ -1294,10 +1299,10 @@
       </c>
       <c r="E20" s="10"/>
       <c r="F20" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G20" s="16">
-        <v>2240</v>
+        <v>8000</v>
       </c>
       <c r="H20" s="16">
         <v>0</v>
@@ -1316,10 +1321,10 @@
       </c>
       <c r="E21" s="10"/>
       <c r="F21" s="17" t="s">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="G21" s="16">
-        <v>0</v>
+        <v>2240</v>
       </c>
       <c r="H21" s="16">
         <v>0</v>
@@ -1327,7 +1332,7 @@
       <c r="I21" s="13"/>
       <c r="J21" s="24"/>
     </row>
-    <row r="22" spans="1:11" s="14" customFormat="1" ht="24.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" s="14" customFormat="1" ht="24.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="18" t="s">
         <v>11</v>
       </c>
@@ -1340,12 +1345,11 @@
         <v>0</v>
       </c>
       <c r="E22" s="10"/>
-      <c r="F22" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="G22" s="21">
-        <f>SUM(G19:G21)</f>
-        <v>10240</v>
+      <c r="F22" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="G22" s="16">
+        <v>0</v>
       </c>
       <c r="H22" s="21">
         <f>SUM(H19:H21)</f>
@@ -1353,14 +1357,19 @@
       </c>
       <c r="I22" s="13"/>
     </row>
-    <row r="23" spans="1:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" ht="24.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B23" s="45"/>
       <c r="C23" s="45"/>
       <c r="D23" s="45"/>
       <c r="E23" s="26"/>
-      <c r="F23" s="44"/>
-      <c r="G23" s="44"/>
-      <c r="H23" s="44"/>
+      <c r="F23" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="G23" s="21">
+        <f>SUM(G20:G22)</f>
+        <v>10240</v>
+      </c>
+      <c r="H23" s="42"/>
     </row>
     <row r="24" spans="1:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="27" t="s">
@@ -1375,13 +1384,8 @@
         <v>0</v>
       </c>
       <c r="E24" s="26"/>
-      <c r="F24" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="G24" s="30">
-        <f>G10+G16+G22</f>
-        <v>23240</v>
-      </c>
+      <c r="F24" s="42"/>
+      <c r="G24" s="42"/>
       <c r="H24" s="30">
         <f>H10+H16+H22</f>
         <v>0</v>
@@ -1394,8 +1398,13 @@
         <v>3</v>
       </c>
       <c r="E25" s="26"/>
-      <c r="F25" s="26"/>
-      <c r="G25" s="26"/>
+      <c r="F25" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="G25" s="30">
+        <f>G11+G17+G23</f>
+        <v>23240</v>
+      </c>
       <c r="H25" s="26"/>
     </row>
     <row r="26" spans="1:11" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
@@ -1403,7 +1412,7 @@
       <c r="C26" s="34"/>
       <c r="D26" s="34"/>
       <c r="E26" s="35"/>
-      <c r="F26" s="35"/>
+      <c r="F26" s="26"/>
       <c r="G26" s="26"/>
       <c r="H26" s="26"/>
     </row>
@@ -1464,14 +1473,14 @@
       <c r="G31" s="26"/>
       <c r="H31" s="26"/>
     </row>
-    <row r="32" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="39"/>
       <c r="B32" s="39"/>
       <c r="C32" s="39"/>
       <c r="D32" s="39"/>
       <c r="E32" s="39"/>
-      <c r="F32" s="39"/>
-      <c r="G32" s="39"/>
+      <c r="F32" s="35"/>
+      <c r="G32" s="26"/>
       <c r="H32" s="39"/>
       <c r="I32" s="39"/>
       <c r="J32" s="39"/>
@@ -2023,12 +2032,13 @@
       <c r="J74" s="39"/>
       <c r="K74" s="39"/>
     </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F75" s="39"/>
+      <c r="G75" s="39"/>
+    </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="4">
     <mergeCell ref="B1:D1"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="F23:H23"/>
     <mergeCell ref="B10:D10"/>
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="B23:D23"/>

</xml_diff>